<commit_message>
[Feat] Geração de arquivo .xlsx com análise
[Feat] Geração de arquivo .xlsx com análise, e tabela na jalena top level
</commit_message>
<xml_diff>
--- a/ParetoExel copy/baseCasos.xlsx
+++ b/ParetoExel copy/baseCasos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="1575" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,13 +16,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -48,9 +53,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,8 +426,8 @@
   </sheetPr>
   <dimension ref="A1:F503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A503"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="C1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -440,22 +446,22 @@
           <t>Preço Errado</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Tipo de Falha</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Nº de Ocorrências</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Fr(%)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Fr Acumulada (%)</t>
         </is>
@@ -651,7 +657,7 @@
           <t>Atraso Transportadora</t>
         </is>
       </c>
-      <c r="C10" s="1" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>Total</t>
         </is>

</xml_diff>